<commit_message>
Updating My excel file
</commit_message>
<xml_diff>
--- a/NewExcel.xlsx
+++ b/NewExcel.xlsx
@@ -16,11 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1" uniqueCount="1">
-  <si>
-    <t>dkjfhsdk</t>
-  </si>
-</sst>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
@@ -357,10 +353,13 @@
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
+  <cols>
+    <col min="4" max="4" width="12" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="2" spans="4:4">
-      <c r="D2" t="s">
-        <v>0</v>
+      <c r="D2">
+        <v>3746283472638430</v>
       </c>
     </row>
   </sheetData>

</xml_diff>